<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@d637c73777c1020575c238a6877a276e93eac622 🚀
</commit_message>
<xml_diff>
--- a/suivis_connaissance.xlsx
+++ b/suivis_connaissance.xlsx
@@ -3212,7 +3212,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3240,7 +3240,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3268,7 +3268,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3296,7 +3296,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3324,7 +3324,7 @@
     <xdr:ext cx="2695575" cy="2695575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image10.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3448,7 +3448,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3476,7 +3476,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3504,7 +3504,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3532,7 +3532,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3560,7 +3560,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3656,7 +3656,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3684,7 +3684,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3712,7 +3712,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3740,7 +3740,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3768,7 +3768,7 @@
     <xdr:ext cx="1143000" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3892,7 +3892,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3920,7 +3920,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3948,7 +3948,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3976,7 +3976,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4004,7 +4004,7 @@
     <xdr:ext cx="1685925" cy="1181100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4128,7 +4128,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4156,7 +4156,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4184,7 +4184,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4212,7 +4212,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4240,7 +4240,7 @@
     <xdr:ext cx="1628775" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4268,7 +4268,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4364,7 +4364,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4392,7 +4392,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4420,7 +4420,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4448,7 +4448,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4476,7 +4476,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4572,7 +4572,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4600,7 +4600,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4628,7 +4628,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4656,7 +4656,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4684,7 +4684,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@ab3c714af3693fc2475e1cd3b6993939007b0f14 🚀
</commit_message>
<xml_diff>
--- a/suivis_connaissance.xlsx
+++ b/suivis_connaissance.xlsx
@@ -3211,7 +3211,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3239,7 +3239,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3267,7 +3267,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3295,7 +3295,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3447,7 +3447,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3475,7 +3475,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3503,7 +3503,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3531,7 +3531,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3655,7 +3655,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3683,7 +3683,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3711,7 +3711,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3739,7 +3739,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3891,7 +3891,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3919,7 +3919,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3947,7 +3947,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3975,7 +3975,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4127,7 +4127,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4155,7 +4155,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4183,7 +4183,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4211,7 +4211,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4363,7 +4363,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4391,7 +4391,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4419,7 +4419,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4447,7 +4447,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@dedb4b157ea8d79f57dfa3ad6cbb084a99715def 🚀
</commit_message>
<xml_diff>
--- a/suivis_connaissance.xlsx
+++ b/suivis_connaissance.xlsx
@@ -3240,7 +3240,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3268,7 +3268,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3324,7 +3324,7 @@
     <xdr:ext cx="2695575" cy="2695575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3352,7 +3352,7 @@
     <xdr:ext cx="1676400" cy="1038225"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.jpg" title="Image"/>
+        <xdr:cNvPr id="0" name="image10.jpg" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3476,7 +3476,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3504,7 +3504,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3560,7 +3560,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3684,7 +3684,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3712,7 +3712,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3768,7 +3768,7 @@
     <xdr:ext cx="1143000" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3796,7 +3796,7 @@
     <xdr:ext cx="2790825" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3920,7 +3920,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3948,7 +3948,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4004,7 +4004,7 @@
     <xdr:ext cx="1685925" cy="1181100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4032,7 +4032,7 @@
     <xdr:ext cx="2800350" cy="2447925"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4156,7 +4156,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4184,7 +4184,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4240,7 +4240,7 @@
     <xdr:ext cx="1628775" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4268,7 +4268,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4392,7 +4392,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4420,7 +4420,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4476,7 +4476,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4600,7 +4600,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4628,7 +4628,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4684,7 +4684,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@95ec715dc7c1380c6ffaa93bd667f9d94355c330 🚀
</commit_message>
<xml_diff>
--- a/suivis_connaissance.xlsx
+++ b/suivis_connaissance.xlsx
@@ -3212,7 +3212,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3268,7 +3268,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3296,7 +3296,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3324,7 +3324,7 @@
     <xdr:ext cx="2695575" cy="2695575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3352,7 +3352,7 @@
     <xdr:ext cx="1676400" cy="1038225"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.jpg" title="Image"/>
+        <xdr:cNvPr id="0" name="image11.jpg" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3448,7 +3448,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3504,7 +3504,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3532,7 +3532,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3560,7 +3560,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3656,7 +3656,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3712,7 +3712,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3740,7 +3740,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3768,7 +3768,7 @@
     <xdr:ext cx="1143000" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3796,7 +3796,7 @@
     <xdr:ext cx="2790825" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3892,7 +3892,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3948,7 +3948,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3976,7 +3976,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4004,7 +4004,7 @@
     <xdr:ext cx="1685925" cy="1181100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4032,7 +4032,7 @@
     <xdr:ext cx="2800350" cy="2447925"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4128,7 +4128,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4184,7 +4184,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4212,7 +4212,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4240,7 +4240,7 @@
     <xdr:ext cx="1628775" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4268,7 +4268,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4364,7 +4364,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4420,7 +4420,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4448,7 +4448,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4476,7 +4476,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4572,7 +4572,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4628,7 +4628,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4656,7 +4656,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4684,7 +4684,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image10.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@6d4b0c08c56445296221594cd8b2280051edf649 🚀
</commit_message>
<xml_diff>
--- a/suivis_connaissance.xlsx
+++ b/suivis_connaissance.xlsx
@@ -3693,7 +3693,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3721,7 +3721,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3777,7 +3777,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3901,7 +3901,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3929,7 +3929,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3985,7 +3985,7 @@
     <xdr:ext cx="1409700" cy="790575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image14.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4013,7 +4013,7 @@
     <xdr:ext cx="2743200" cy="2743200"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image13.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4137,7 +4137,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4165,7 +4165,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4345,7 +4345,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4373,7 +4373,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4429,7 +4429,7 @@
     <xdr:ext cx="2695575" cy="2695575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4457,7 +4457,7 @@
     <xdr:ext cx="1676400" cy="1038225"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.jpg" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.jpg" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4581,7 +4581,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4609,7 +4609,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4665,7 +4665,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4789,7 +4789,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4817,7 +4817,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4901,7 +4901,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5025,7 +5025,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5053,7 +5053,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5261,7 +5261,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5289,7 +5289,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5345,7 +5345,7 @@
     <xdr:ext cx="1143000" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image13.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5373,7 +5373,7 @@
     <xdr:ext cx="2790825" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@f2b1592ee9c761457cb015e1dd04606847d83701 🚀
</commit_message>
<xml_diff>
--- a/suivis_connaissance.xlsx
+++ b/suivis_connaissance.xlsx
@@ -3665,7 +3665,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3693,7 +3693,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3721,7 +3721,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3749,7 +3749,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3777,7 +3777,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3873,7 +3873,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3901,7 +3901,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3929,7 +3929,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3957,7 +3957,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3985,7 +3985,7 @@
     <xdr:ext cx="1409700" cy="790575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image13.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4013,7 +4013,7 @@
     <xdr:ext cx="2743200" cy="2743200"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image13.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image14.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4109,7 +4109,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4137,7 +4137,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4165,7 +4165,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4193,7 +4193,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4317,7 +4317,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4345,7 +4345,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4373,7 +4373,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4401,7 +4401,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4457,7 +4457,7 @@
     <xdr:ext cx="1676400" cy="1038225"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.jpg" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4553,7 +4553,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4581,7 +4581,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4609,7 +4609,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4637,7 +4637,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4665,7 +4665,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4761,7 +4761,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4789,7 +4789,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4817,7 +4817,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4845,7 +4845,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4873,7 +4873,7 @@
     <xdr:ext cx="1628775" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4901,7 +4901,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4997,7 +4997,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5025,7 +5025,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5053,7 +5053,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5081,7 +5081,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5137,7 +5137,7 @@
     <xdr:ext cx="2800350" cy="2447925"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5233,7 +5233,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5261,7 +5261,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5289,7 +5289,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5317,7 +5317,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@fd5da14fc30a0c0213af4479ce48284b68b23fa1 🚀
</commit_message>
<xml_diff>
--- a/suivis_connaissance.xlsx
+++ b/suivis_connaissance.xlsx
@@ -3693,7 +3693,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3721,7 +3721,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3901,7 +3901,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3929,7 +3929,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4137,7 +4137,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4165,7 +4165,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4345,7 +4345,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4373,7 +4373,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4581,7 +4581,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4609,7 +4609,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4789,7 +4789,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4817,7 +4817,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5025,7 +5025,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5053,7 +5053,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5261,7 +5261,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5289,7 +5289,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5345,7 +5345,7 @@
     <xdr:ext cx="1143000" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5373,7 +5373,7 @@
     <xdr:ext cx="2790825" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@a1c375a647d429daefb2bfaf2c6ac54a19852781 🚀
</commit_message>
<xml_diff>
--- a/suivis_connaissance.xlsx
+++ b/suivis_connaissance.xlsx
@@ -3665,7 +3665,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3721,7 +3721,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3749,7 +3749,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3777,7 +3777,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3873,7 +3873,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3929,7 +3929,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3957,7 +3957,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3985,7 +3985,7 @@
     <xdr:ext cx="1409700" cy="790575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image13.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4013,7 +4013,7 @@
     <xdr:ext cx="2743200" cy="2743200"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image13.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image14.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4109,7 +4109,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4165,7 +4165,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4193,7 +4193,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4221,7 +4221,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4317,7 +4317,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4373,7 +4373,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4401,7 +4401,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4429,7 +4429,7 @@
     <xdr:ext cx="2695575" cy="2695575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4457,7 +4457,7 @@
     <xdr:ext cx="1676400" cy="1038225"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.jpg" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4553,7 +4553,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4609,7 +4609,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4637,7 +4637,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4665,7 +4665,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4761,7 +4761,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4817,7 +4817,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4845,7 +4845,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4873,7 +4873,7 @@
     <xdr:ext cx="1628775" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image10.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4901,7 +4901,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4997,7 +4997,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5053,7 +5053,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5081,7 +5081,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5109,7 +5109,7 @@
     <xdr:ext cx="1685925" cy="1181100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5137,7 +5137,7 @@
     <xdr:ext cx="2800350" cy="2447925"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5233,7 +5233,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5289,7 +5289,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5317,7 +5317,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5345,7 +5345,7 @@
     <xdr:ext cx="1143000" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5373,7 +5373,7 @@
     <xdr:ext cx="2790825" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@77a903707b962218897510fb7308edaa7ba88d51 🚀
</commit_message>
<xml_diff>
--- a/suivis_connaissance.xlsx
+++ b/suivis_connaissance.xlsx
@@ -3665,7 +3665,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3693,7 +3693,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3721,7 +3721,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3749,7 +3749,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3777,7 +3777,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3873,7 +3873,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3901,7 +3901,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3929,7 +3929,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3957,7 +3957,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3985,7 +3985,7 @@
     <xdr:ext cx="1409700" cy="790575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image13.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image10.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4013,7 +4013,7 @@
     <xdr:ext cx="2743200" cy="2743200"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4109,7 +4109,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4137,7 +4137,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4165,7 +4165,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4193,7 +4193,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4317,7 +4317,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4345,7 +4345,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4373,7 +4373,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4401,7 +4401,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4429,7 +4429,7 @@
     <xdr:ext cx="2695575" cy="2695575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4457,7 +4457,7 @@
     <xdr:ext cx="1676400" cy="1038225"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.jpg" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.jpg" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4553,7 +4553,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4581,7 +4581,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4609,7 +4609,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4637,7 +4637,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4665,7 +4665,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4761,7 +4761,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4789,7 +4789,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4817,7 +4817,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4845,7 +4845,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4873,7 +4873,7 @@
     <xdr:ext cx="1628775" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4901,7 +4901,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4997,7 +4997,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5025,7 +5025,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5053,7 +5053,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5081,7 +5081,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5109,7 +5109,7 @@
     <xdr:ext cx="1685925" cy="1181100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image13.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5137,7 +5137,7 @@
     <xdr:ext cx="2800350" cy="2447925"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5233,7 +5233,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5261,7 +5261,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5289,7 +5289,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5317,7 +5317,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5345,7 +5345,7 @@
     <xdr:ext cx="1143000" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image14.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5373,7 +5373,7 @@
     <xdr:ext cx="2790825" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@1290c7654c53dc107a4fc32ee1aa61dc0a40c5ad 🚀
</commit_message>
<xml_diff>
--- a/suivis_connaissance.xlsx
+++ b/suivis_connaissance.xlsx
@@ -3665,7 +3665,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3693,7 +3693,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3721,7 +3721,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3749,7 +3749,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3777,7 +3777,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3873,7 +3873,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3901,7 +3901,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3929,7 +3929,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3957,7 +3957,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3985,7 +3985,7 @@
     <xdr:ext cx="1409700" cy="790575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image14.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4013,7 +4013,7 @@
     <xdr:ext cx="2743200" cy="2743200"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image13.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4109,7 +4109,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4137,7 +4137,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4165,7 +4165,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4193,7 +4193,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4221,7 +4221,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4317,7 +4317,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4345,7 +4345,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4373,7 +4373,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4401,7 +4401,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4429,7 +4429,7 @@
     <xdr:ext cx="2695575" cy="2695575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4457,7 +4457,7 @@
     <xdr:ext cx="1676400" cy="1038225"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.jpg" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4553,7 +4553,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4581,7 +4581,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4609,7 +4609,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4637,7 +4637,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4665,7 +4665,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4761,7 +4761,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4789,7 +4789,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4817,7 +4817,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4845,7 +4845,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4873,7 +4873,7 @@
     <xdr:ext cx="1628775" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4901,7 +4901,7 @@
     <xdr:ext cx="2762250" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4997,7 +4997,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5025,7 +5025,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5053,7 +5053,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5081,7 +5081,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5109,7 +5109,7 @@
     <xdr:ext cx="1685925" cy="1181100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image13.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5137,7 +5137,7 @@
     <xdr:ext cx="2800350" cy="2447925"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image10.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5233,7 +5233,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5261,7 +5261,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5289,7 +5289,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5317,7 +5317,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5345,7 +5345,7 @@
     <xdr:ext cx="1143000" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5373,7 +5373,7 @@
     <xdr:ext cx="2790825" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@4b68647e99af7959d1d4d26a67b5e447ca72a553 🚀
</commit_message>
<xml_diff>
--- a/suivis_connaissance.xlsx
+++ b/suivis_connaissance.xlsx
@@ -790,7 +790,8 @@
   </si>
   <si>
     <t>Suivi de l'évolution de la répartition et précision des limites de l'aire de répartition en Île-de-France.
-Etude de l'hybridation avec le chat domestique.</t>
+Etude de l'hybridation avec le chat domestique.
+Evaluation des continuité écologiques pour l'espèce</t>
   </si>
   <si>
     <r>
@@ -3330,6 +3331,9 @@
     <xf borderId="45" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="41" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="13" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -3347,9 +3351,6 @@
     </xf>
     <xf borderId="27" fillId="4" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="41" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="27" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -3665,7 +3666,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3721,7 +3722,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3749,7 +3750,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3873,7 +3874,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3929,7 +3930,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3957,7 +3958,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3985,7 +3986,7 @@
     <xdr:ext cx="1409700" cy="790575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4109,7 +4110,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4165,7 +4166,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4193,7 +4194,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4317,7 +4318,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4373,7 +4374,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4401,7 +4402,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4553,7 +4554,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4609,7 +4610,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4637,7 +4638,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4761,7 +4762,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4817,7 +4818,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4845,7 +4846,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4873,7 +4874,7 @@
     <xdr:ext cx="1628775" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image14.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4997,7 +4998,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5053,7 +5054,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5081,7 +5082,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5109,7 +5110,7 @@
     <xdr:ext cx="1685925" cy="1181100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5137,7 +5138,7 @@
     <xdr:ext cx="2800350" cy="2447925"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5233,7 +5234,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5289,7 +5290,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5317,7 +5318,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5345,7 +5346,7 @@
     <xdr:ext cx="1143000" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image10.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5373,7 +5374,7 @@
     <xdr:ext cx="2790825" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5965,7 +5966,7 @@
       <c r="B12" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="81" t="s">
+      <c r="C12" s="132" t="s">
         <v>104</v>
       </c>
       <c r="D12" s="63"/>
@@ -6434,7 +6435,7 @@
       </c>
       <c r="Q29" s="8"/>
       <c r="R29" s="18"/>
-      <c r="S29" s="132" t="inlineStr">
+      <c r="S29" s="133" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -6468,7 +6469,7 @@
       </c>
       <c r="Q30" s="8"/>
       <c r="R30" s="18"/>
-      <c r="S30" s="132" t="inlineStr">
+      <c r="S30" s="133" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -6984,7 +6985,7 @@
       <c r="D47" s="96"/>
       <c r="E47" s="96"/>
       <c r="F47" s="97"/>
-      <c r="G47" s="133" t="inlineStr">
+      <c r="G47" s="134" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -7001,7 +7002,7 @@
       </c>
       <c r="N47" s="8"/>
       <c r="O47" s="18"/>
-      <c r="P47" s="134" t="inlineStr">
+      <c r="P47" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -7028,7 +7029,7 @@
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="18"/>
-      <c r="G48" s="134" t="inlineStr">
+      <c r="G48" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -7043,7 +7044,7 @@
       </c>
       <c r="N48" s="8"/>
       <c r="O48" s="18"/>
-      <c r="P48" s="134" t="inlineStr">
+      <c r="P48" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -7062,7 +7063,7 @@
       <c r="AB48" s="38"/>
     </row>
     <row customHeight="1" ht="15.75" r="49">
-      <c r="A49" s="135">
+      <c r="A49" s="136">
         <v>45743.0</v>
       </c>
       <c r="B49" s="18"/>
@@ -7072,7 +7073,7 @@
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
       <c r="F49" s="18"/>
-      <c r="G49" s="134" t="inlineStr">
+      <c r="G49" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -7087,7 +7088,7 @@
       </c>
       <c r="N49" s="8"/>
       <c r="O49" s="18"/>
-      <c r="P49" s="136" t="inlineStr">
+      <c r="P49" s="137" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -13416,7 +13417,7 @@
       <c r="M6" s="128" t="s">
         <v>98</v>
       </c>
-      <c r="N6" s="137">
+      <c r="N6" s="138">
         <v>45689.0</v>
       </c>
       <c r="O6" s="36"/>
@@ -13604,7 +13605,7 @@
       <c r="B12" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="138" t="s">
+      <c r="C12" s="132" t="s">
         <v>135</v>
       </c>
       <c r="D12" s="63"/>
@@ -13722,7 +13723,7 @@
       <c r="B16" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="138" t="s">
+      <c r="C16" s="132" t="s">
         <v>137</v>
       </c>
       <c r="D16" s="63"/>
@@ -14073,7 +14074,7 @@
       </c>
       <c r="Q29" s="8"/>
       <c r="R29" s="18"/>
-      <c r="S29" s="132" t="inlineStr">
+      <c r="S29" s="133" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -14621,7 +14622,7 @@
       <c r="D47" s="96"/>
       <c r="E47" s="96"/>
       <c r="F47" s="97"/>
-      <c r="G47" s="133" t="inlineStr">
+      <c r="G47" s="134" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -14638,7 +14639,7 @@
       </c>
       <c r="N47" s="8"/>
       <c r="O47" s="18"/>
-      <c r="P47" s="134" t="inlineStr">
+      <c r="P47" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -14665,7 +14666,7 @@
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="18"/>
-      <c r="G48" s="134" t="inlineStr">
+      <c r="G48" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -14680,7 +14681,7 @@
       </c>
       <c r="N48" s="8"/>
       <c r="O48" s="18"/>
-      <c r="P48" s="134" t="inlineStr">
+      <c r="P48" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -14699,7 +14700,7 @@
       <c r="AB48" s="38"/>
     </row>
     <row customHeight="1" ht="15.75" r="49">
-      <c r="A49" s="135">
+      <c r="A49" s="136">
         <v>45743.0</v>
       </c>
       <c r="B49" s="18"/>
@@ -14718,7 +14719,7 @@
       </c>
       <c r="N49" s="8"/>
       <c r="O49" s="18"/>
-      <c r="P49" s="134" t="inlineStr">
+      <c r="P49" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -21352,7 +21353,7 @@
       <c r="B16" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="138" t="s">
+      <c r="C16" s="132" t="s">
         <v>163</v>
       </c>
       <c r="D16" s="63"/>
@@ -21733,7 +21734,7 @@
       </c>
       <c r="Q30" s="8"/>
       <c r="R30" s="18"/>
-      <c r="S30" s="132" t="inlineStr">
+      <c r="S30" s="133" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -22263,7 +22264,7 @@
       <c r="D47" s="96"/>
       <c r="E47" s="96"/>
       <c r="F47" s="97"/>
-      <c r="G47" s="133" t="inlineStr">
+      <c r="G47" s="134" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -22280,7 +22281,7 @@
       </c>
       <c r="N47" s="8"/>
       <c r="O47" s="18"/>
-      <c r="P47" s="134" t="inlineStr">
+      <c r="P47" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -22335,7 +22336,7 @@
       <c r="AB48" s="38"/>
     </row>
     <row customHeight="1" ht="15.75" r="49">
-      <c r="A49" s="135">
+      <c r="A49" s="136">
         <v>45743.0</v>
       </c>
       <c r="B49" s="18"/>
@@ -29330,7 +29331,7 @@
       </c>
       <c r="Q29" s="8"/>
       <c r="R29" s="18"/>
-      <c r="S29" s="132" t="inlineStr">
+      <c r="S29" s="133" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -29892,7 +29893,7 @@
       <c r="D47" s="96"/>
       <c r="E47" s="96"/>
       <c r="F47" s="97"/>
-      <c r="G47" s="133" t="inlineStr">
+      <c r="G47" s="134" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -29936,7 +29937,7 @@
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="18"/>
-      <c r="G48" s="134" t="inlineStr">
+      <c r="G48" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -29970,7 +29971,7 @@
       <c r="AB48" s="38"/>
     </row>
     <row customHeight="1" ht="15.75" r="49">
-      <c r="A49" s="135">
+      <c r="A49" s="136">
         <v>45743.0</v>
       </c>
       <c r="B49" s="18"/>
@@ -37537,7 +37538,7 @@
       <c r="D47" s="96"/>
       <c r="E47" s="96"/>
       <c r="F47" s="97"/>
-      <c r="G47" s="133" t="inlineStr">
+      <c r="G47" s="134" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -37554,7 +37555,7 @@
       </c>
       <c r="N47" s="8"/>
       <c r="O47" s="18"/>
-      <c r="P47" s="136" t="inlineStr">
+      <c r="P47" s="137" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -37581,7 +37582,7 @@
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="18"/>
-      <c r="G48" s="134" t="inlineStr">
+      <c r="G48" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -37615,7 +37616,7 @@
       <c r="AB48" s="38"/>
     </row>
     <row customHeight="1" ht="15.75" r="49">
-      <c r="A49" s="135">
+      <c r="A49" s="136">
         <v>45743.0</v>
       </c>
       <c r="B49" s="18"/>
@@ -44618,7 +44619,7 @@
       </c>
       <c r="Q29" s="8"/>
       <c r="R29" s="18"/>
-      <c r="S29" s="132" t="inlineStr">
+      <c r="S29" s="133" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -44652,7 +44653,7 @@
       </c>
       <c r="Q30" s="8"/>
       <c r="R30" s="18"/>
-      <c r="S30" s="132" t="inlineStr">
+      <c r="S30" s="133" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -44686,7 +44687,7 @@
       </c>
       <c r="Q31" s="8"/>
       <c r="R31" s="18"/>
-      <c r="S31" s="132" t="inlineStr">
+      <c r="S31" s="133" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -44744,7 +44745,7 @@
       </c>
       <c r="Q33" s="8"/>
       <c r="R33" s="18"/>
-      <c r="S33" s="132" t="inlineStr">
+      <c r="S33" s="133" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -45233,7 +45234,7 @@
       </c>
       <c r="N47" s="8"/>
       <c r="O47" s="18"/>
-      <c r="P47" s="134" t="inlineStr">
+      <c r="P47" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -45260,7 +45261,7 @@
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="18"/>
-      <c r="G48" s="134" t="inlineStr">
+      <c r="G48" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -45275,7 +45276,7 @@
       </c>
       <c r="N48" s="8"/>
       <c r="O48" s="18"/>
-      <c r="P48" s="134" t="inlineStr">
+      <c r="P48" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -45294,7 +45295,7 @@
       <c r="AB48" s="38"/>
     </row>
     <row customHeight="1" ht="15.75" r="49">
-      <c r="A49" s="135">
+      <c r="A49" s="136">
         <v>45743.0</v>
       </c>
       <c r="B49" s="18"/>
@@ -45304,7 +45305,7 @@
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
       <c r="F49" s="18"/>
-      <c r="G49" s="134" t="inlineStr">
+      <c r="G49" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -45319,7 +45320,7 @@
       </c>
       <c r="N49" s="8"/>
       <c r="O49" s="18"/>
-      <c r="P49" s="134" t="inlineStr">
+      <c r="P49" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -52307,7 +52308,7 @@
       </c>
       <c r="Q29" s="8"/>
       <c r="R29" s="18"/>
-      <c r="S29" s="132" t="inlineStr">
+      <c r="S29" s="133" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -52887,7 +52888,7 @@
       <c r="D47" s="96"/>
       <c r="E47" s="96"/>
       <c r="F47" s="97"/>
-      <c r="G47" s="133" t="inlineStr">
+      <c r="G47" s="134" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -52931,7 +52932,7 @@
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="18"/>
-      <c r="G48" s="134" t="inlineStr">
+      <c r="G48" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -52946,7 +52947,7 @@
       </c>
       <c r="N48" s="8"/>
       <c r="O48" s="18"/>
-      <c r="P48" s="134" t="inlineStr">
+      <c r="P48" s="135" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -52965,7 +52966,7 @@
       <c r="AB48" s="38"/>
     </row>
     <row customHeight="1" ht="15.75" r="49">
-      <c r="A49" s="135">
+      <c r="A49" s="136">
         <v>45743.0</v>
       </c>
       <c r="B49" s="18"/>
@@ -59493,7 +59494,7 @@
       <c r="B12" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="138" t="s">
+      <c r="C12" s="132" t="s">
         <v>299</v>
       </c>
       <c r="D12" s="63"/>
@@ -60601,7 +60602,7 @@
       </c>
       <c r="N48" s="8"/>
       <c r="O48" s="18"/>
-      <c r="P48" s="136" t="inlineStr">
+      <c r="P48" s="137" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -60645,7 +60646,7 @@
       </c>
       <c r="N49" s="8"/>
       <c r="O49" s="18"/>
-      <c r="P49" s="136" t="inlineStr">
+      <c r="P49" s="137" t="inlineStr">
         <is>
           <t/>
         </is>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@722e7fc242599d439fa74ebf1b4ba56fe310d6de 🚀
</commit_message>
<xml_diff>
--- a/suivis_connaissance.xlsx
+++ b/suivis_connaissance.xlsx
@@ -3666,7 +3666,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3694,7 +3694,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3750,7 +3750,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3874,7 +3874,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3902,7 +3902,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3958,7 +3958,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4110,7 +4110,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4138,7 +4138,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4194,7 +4194,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4318,7 +4318,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4346,7 +4346,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4402,7 +4402,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4554,7 +4554,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4582,7 +4582,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4638,7 +4638,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4762,7 +4762,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4790,7 +4790,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4846,7 +4846,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4998,7 +4998,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5026,7 +5026,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5082,7 +5082,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5234,7 +5234,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5262,7 +5262,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5318,7 +5318,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5346,7 +5346,7 @@
     <xdr:ext cx="1143000" cy="1143000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5374,7 +5374,7 @@
     <xdr:ext cx="2790825" cy="2400300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@fcfefb60962d00eb43f056fb2d16f8c92ba52015 🚀
</commit_message>
<xml_diff>
--- a/suivis_connaissance.xlsx
+++ b/suivis_connaissance.xlsx
@@ -3666,7 +3666,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3694,7 +3694,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3722,7 +3722,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3750,7 +3750,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3874,7 +3874,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3902,7 +3902,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3930,7 +3930,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3958,7 +3958,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4110,7 +4110,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4138,7 +4138,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4166,7 +4166,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4194,7 +4194,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4318,7 +4318,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4346,7 +4346,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4374,7 +4374,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4402,7 +4402,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4554,7 +4554,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4582,7 +4582,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4610,7 +4610,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4638,7 +4638,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4762,7 +4762,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4790,7 +4790,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4818,7 +4818,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4846,7 +4846,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4998,7 +4998,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5026,7 +5026,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5054,7 +5054,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5082,7 +5082,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5234,7 +5234,7 @@
     <xdr:ext cx="1276350" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5262,7 +5262,7 @@
     <xdr:ext cx="390525" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5290,7 +5290,7 @@
     <xdr:ext cx="504825" cy="409575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5318,7 +5318,7 @@
     <xdr:ext cx="1257300" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>